<commit_message>
import gst data add
</commit_message>
<xml_diff>
--- a/gst_tax_data.xlsx
+++ b/gst_tax_data.xlsx
@@ -1,34 +1,148 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Python\GST Billing\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{752C544A-0C3D-4D47-83C4-B89E5A6E31FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Phone no</t>
+  </si>
+  <si>
+    <t>GSTIN no</t>
+  </si>
+  <si>
+    <t>Business Type</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Email ID</t>
+  </si>
+  <si>
+    <t>Billing Address</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Pay Balance</t>
+  </si>
+  <si>
+    <t>Received Balance</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Unregistered/Consumer</t>
+  </si>
+  <si>
+    <t>Eegistered Business - Regular</t>
+  </si>
+  <si>
+    <t>Eegistered Business - Composition</t>
+  </si>
+  <si>
+    <t>Tom Smith</t>
+  </si>
+  <si>
+    <t>john@example.com</t>
+  </si>
+  <si>
+    <t>jane@example.com</t>
+  </si>
+  <si>
+    <t>mike@example.com</t>
+  </si>
+  <si>
+    <t>123 Main St</t>
+  </si>
+  <si>
+    <t>456 Oak Ave</t>
+  </si>
+  <si>
+    <t>789 Elm St, Dallas</t>
+  </si>
+  <si>
+    <t>123 Main St, New York</t>
+  </si>
+  <si>
+    <t>456 Oak Ave, Los Angeles</t>
+  </si>
+  <si>
+    <t>Maharashtra</t>
+  </si>
+  <si>
+    <t>Goa</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -43,84 +157,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -408,99 +468,163 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Name</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>Tax Amount</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>GST Rate</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>GST Amount</t>
-        </is>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Mike Johnson</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
         <v>800</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>05</t>
-        </is>
-      </c>
-      <c r="D2">
-        <f>B4*C4/100</f>
-        <v/>
+      <c r="C2">
+        <v>1562485262</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2">
+        <v>1000</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>44562</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Jane Smith</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>1500</v>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="D3">
-        <f>B3*C3/100</f>
-        <v/>
+      <c r="C3">
+        <v>1215264525</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3">
+        <v>4562</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="3">
+        <v>44607</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>John Doe</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>1000</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
-      </c>
-      <c r="D4">
-        <f>B2*C2/100</f>
-        <v/>
+      <c r="C4">
+        <v>1845962135</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>4200</v>
+      </c>
+      <c r="K4" s="3">
+        <v>44650</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{F015FF6C-A874-4144-ADF8-7A44D8D914C0}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{9516B6BE-B70B-480F-A700-05AF05B2EE1E}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{F0F86FAB-75DA-48CE-9D39-CB0E7534D484}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>